<commit_message>
added all cleaned data files
</commit_message>
<xml_diff>
--- a/data/per_100_posessions_historical.xlsx
+++ b/data/per_100_posessions_historical.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taajcheema/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0E181BD-0F78-304F-A0C3-EBF765528669}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB522678-4E06-AA42-8422-A23077950903}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="460" windowWidth="27600" windowHeight="17040" xr2:uid="{3100F5C7-0A2C-CA46-9F76-84D8F260537E}"/>
   </bookViews>
@@ -193,7 +193,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -202,16 +202,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="9.4"/>
-      <color rgb="FF990000"/>
-      <name val="Verdana"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9.4"/>
-      <color rgb="FF000000"/>
-      <name val="Verdana"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -220,7 +221,19 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -242,19 +255,20 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -570,2017 +584,2199 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB3D43B-889E-A543-A442-89C661BE3959}">
-  <dimension ref="A1:AE25"/>
+  <dimension ref="A1:AF26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:32">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:32">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>26</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="4">
         <v>216</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="4">
         <v>971</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="4">
         <v>40.5</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="4">
         <v>88</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="4">
         <v>12</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="4">
         <v>33.6</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="4">
         <v>17.5</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="4">
         <v>22.7</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="4">
         <v>10</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="4">
         <v>34.4</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="4">
         <v>44.5</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="4">
         <v>24.1</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="4">
         <v>7.6</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="4">
         <v>4.9000000000000004</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="4">
         <v>14.4</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="4">
         <v>20.399999999999999</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="4">
         <v>110.4</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2" s="4">
         <v>0.46</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2" s="4">
         <v>0.35699999999999998</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Y2" s="4">
         <v>0.77100000000000002</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="Z2" s="4">
         <v>100.2</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AA2" s="4">
         <v>0.52800000000000002</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AB2" s="4">
         <v>12.8</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AC2" s="4">
         <v>22.6</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AD2" s="4">
         <v>0.19900000000000001</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="AE2" s="4">
         <v>110.4</v>
       </c>
+      <c r="AF2" s="1"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    <row r="3" spans="1:32">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>26.3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="4">
         <v>217</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="4">
         <v>1230</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="4">
         <v>40.799999999999997</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="4">
         <v>88.6</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="4">
         <v>11.3</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="4">
         <v>31.8</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="4">
         <v>17.600000000000001</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="4">
         <v>22.9</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="4">
         <v>10.3</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="4">
         <v>34.6</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="4">
         <v>44.8</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="4">
         <v>24.4</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="4">
         <v>7.6</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="4">
         <v>4.9000000000000004</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T3" s="4">
         <v>14</v>
       </c>
-      <c r="U3" s="2">
+      <c r="U3" s="4">
         <v>20.8</v>
       </c>
-      <c r="V3" s="2">
+      <c r="V3" s="4">
         <v>110.4</v>
       </c>
-      <c r="W3" s="2">
+      <c r="W3" s="4">
         <v>0.46100000000000002</v>
       </c>
-      <c r="X3" s="2">
+      <c r="X3" s="4">
         <v>0.35499999999999998</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="Y3" s="4">
         <v>0.76600000000000001</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="Z3" s="4">
         <v>100</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AA3" s="4">
         <v>0.52400000000000002</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AB3" s="4">
         <v>12.4</v>
       </c>
-      <c r="AC3" s="2">
+      <c r="AC3" s="4">
         <v>22.9</v>
       </c>
-      <c r="AD3" s="2">
+      <c r="AD3" s="4">
         <v>0.19800000000000001</v>
       </c>
-      <c r="AE3" s="2">
+      <c r="AE3" s="4">
         <v>110.4</v>
       </c>
+      <c r="AF3" s="1"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="4" spans="1:32">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>26.4</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <v>219</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="4">
         <v>1230</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="4">
         <v>40.5</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="4">
         <v>87.9</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="4">
         <v>10.7</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="4">
         <v>29.6</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="4">
         <v>17</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="4">
         <v>22.1</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="4">
         <v>9.9</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="4">
         <v>34.5</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="4">
         <v>44.4</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="4">
         <v>23.7</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="4">
         <v>7.9</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="4">
         <v>4.9000000000000004</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4" s="4">
         <v>14.6</v>
       </c>
-      <c r="U4" s="2">
+      <c r="U4" s="4">
         <v>20.3</v>
       </c>
-      <c r="V4" s="2">
+      <c r="V4" s="4">
         <v>108.6</v>
       </c>
-      <c r="W4" s="2">
+      <c r="W4" s="4">
         <v>0.46</v>
       </c>
-      <c r="X4" s="2">
+      <c r="X4" s="4">
         <v>0.36199999999999999</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="Y4" s="4">
         <v>0.76700000000000002</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="Z4" s="4">
         <v>97.3</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AA4" s="4">
         <v>0.52100000000000002</v>
       </c>
-      <c r="AB4" s="2">
+      <c r="AB4" s="4">
         <v>13</v>
       </c>
-      <c r="AC4" s="2">
+      <c r="AC4" s="4">
         <v>22.3</v>
       </c>
-      <c r="AD4" s="2">
+      <c r="AD4" s="4">
         <v>0.193</v>
       </c>
-      <c r="AE4" s="2">
+      <c r="AE4" s="4">
         <v>108.6</v>
       </c>
+      <c r="AF4" s="1"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5" spans="1:32">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>26.6</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="4">
         <v>220</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="4">
         <v>1230</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="4">
         <v>40.200000000000003</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="4">
         <v>88</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="4">
         <v>9.9</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="4">
         <v>27.8</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="4">
         <v>18.399999999999999</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="4">
         <v>23.8</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="4">
         <v>10.4</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="4">
         <v>34.4</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="4">
         <v>44.8</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="4">
         <v>23.3</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="4">
         <v>7.9</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="4">
         <v>4.9000000000000004</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5" s="4">
         <v>14.4</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5" s="4">
         <v>20.5</v>
       </c>
-      <c r="V5" s="2">
+      <c r="V5" s="4">
         <v>108.8</v>
       </c>
-      <c r="W5" s="2">
+      <c r="W5" s="4">
         <v>0.45700000000000002</v>
       </c>
-      <c r="X5" s="2">
+      <c r="X5" s="4">
         <v>0.35799999999999998</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="Y5" s="4">
         <v>0.77200000000000002</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="Z5" s="4">
         <v>96.4</v>
       </c>
-      <c r="AA5" s="2">
+      <c r="AA5" s="4">
         <v>0.51400000000000001</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="AB5" s="4">
         <v>12.7</v>
       </c>
-      <c r="AC5" s="2">
+      <c r="AC5" s="4">
         <v>23.3</v>
       </c>
-      <c r="AD5" s="2">
+      <c r="AD5" s="4">
         <v>0.20899999999999999</v>
       </c>
-      <c r="AE5" s="2">
+      <c r="AE5" s="4">
         <v>108.8</v>
       </c>
+      <c r="AF5" s="1"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+    <row r="6" spans="1:32">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>26.7</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="4">
         <v>221</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="4">
         <v>1230</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="4">
         <v>39.6</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="4">
         <v>87.6</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="4">
         <v>8.8000000000000007</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="4">
         <v>25</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="4">
         <v>18.3</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="4">
         <v>24.2</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="4">
         <v>10.8</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="4">
         <v>34.6</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="4">
         <v>45.3</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="4">
         <v>23.1</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6" s="4">
         <v>8.1</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6" s="4">
         <v>5.0999999999999996</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T6" s="4">
         <v>14.9</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U6" s="4">
         <v>21</v>
       </c>
-      <c r="V6" s="2">
+      <c r="V6" s="4">
         <v>106.4</v>
       </c>
-      <c r="W6" s="2">
+      <c r="W6" s="4">
         <v>0.45200000000000001</v>
       </c>
-      <c r="X6" s="2">
+      <c r="X6" s="4">
         <v>0.35399999999999998</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="Y6" s="4">
         <v>0.75700000000000001</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="Z6" s="4">
         <v>95.8</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="AA6" s="4">
         <v>0.502</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="AB6" s="4">
         <v>13.2</v>
       </c>
-      <c r="AC6" s="2">
+      <c r="AC6" s="4">
         <v>23.8</v>
       </c>
-      <c r="AD6" s="2">
+      <c r="AD6" s="4">
         <v>0.20899999999999999</v>
       </c>
-      <c r="AE6" s="2">
+      <c r="AE6" s="4">
         <v>106.4</v>
       </c>
+      <c r="AF6" s="1"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+    <row r="7" spans="1:32">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>26.7</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="4">
         <v>222</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="4">
         <v>1230</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="4">
         <v>39.6</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="4">
         <v>88.3</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="4">
         <v>8.3000000000000007</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="4">
         <v>23.7</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="4">
         <v>18.100000000000001</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="4">
         <v>24.1</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="4">
         <v>11.5</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="4">
         <v>34.200000000000003</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="4">
         <v>45.7</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="Q7" s="4">
         <v>23.3</v>
       </c>
-      <c r="R7" s="2">
+      <c r="R7" s="4">
         <v>8.1999999999999993</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7" s="4">
         <v>5.0999999999999996</v>
       </c>
-      <c r="T7" s="2">
+      <c r="T7" s="4">
         <v>15.2</v>
       </c>
-      <c r="U7" s="2">
+      <c r="U7" s="4">
         <v>21.4</v>
       </c>
-      <c r="V7" s="2">
+      <c r="V7" s="4">
         <v>105.6</v>
       </c>
-      <c r="W7" s="2">
+      <c r="W7" s="4">
         <v>0.44900000000000001</v>
       </c>
-      <c r="X7" s="2">
+      <c r="X7" s="4">
         <v>0.35</v>
       </c>
-      <c r="Y7" s="2">
+      <c r="Y7" s="4">
         <v>0.75</v>
       </c>
-      <c r="Z7" s="2">
+      <c r="Z7" s="4">
         <v>93.9</v>
       </c>
-      <c r="AA7" s="2">
+      <c r="AA7" s="4">
         <v>0.496</v>
       </c>
-      <c r="AB7" s="2">
+      <c r="AB7" s="4">
         <v>13.3</v>
       </c>
-      <c r="AC7" s="2">
+      <c r="AC7" s="4">
         <v>25.1</v>
       </c>
-      <c r="AD7" s="2">
+      <c r="AD7" s="4">
         <v>0.20499999999999999</v>
       </c>
-      <c r="AE7" s="2">
+      <c r="AE7" s="4">
         <v>105.6</v>
       </c>
+      <c r="AF7" s="1"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+    <row r="8" spans="1:32">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <v>26.5</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="4">
         <v>223</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="4">
         <v>1230</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="4">
         <v>39.799999999999997</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="4">
         <v>87.6</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="4">
         <v>8.1999999999999993</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="4">
         <v>22.7</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="4">
         <v>18.8</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="4">
         <v>24.9</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="4">
         <v>11.5</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="4">
         <v>33.6</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="4">
         <v>45.1</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="Q8" s="4">
         <v>23.2</v>
       </c>
-      <c r="R8" s="2">
+      <c r="R8" s="4">
         <v>8.1</v>
       </c>
-      <c r="S8" s="2">
+      <c r="S8" s="4">
         <v>5</v>
       </c>
-      <c r="T8" s="2">
+      <c r="T8" s="4">
         <v>15.5</v>
       </c>
-      <c r="U8" s="2">
+      <c r="U8" s="4">
         <v>21.9</v>
       </c>
-      <c r="V8" s="2">
+      <c r="V8" s="4">
         <v>106.6</v>
       </c>
-      <c r="W8" s="2">
+      <c r="W8" s="4">
         <v>0.45400000000000001</v>
       </c>
-      <c r="X8" s="2">
+      <c r="X8" s="4">
         <v>0.36</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="Y8" s="4">
         <v>0.75600000000000001</v>
       </c>
-      <c r="Z8" s="2">
+      <c r="Z8" s="4">
         <v>93.9</v>
       </c>
-      <c r="AA8" s="2">
+      <c r="AA8" s="4">
         <v>0.501</v>
       </c>
-      <c r="AB8" s="2">
+      <c r="AB8" s="4">
         <v>13.6</v>
       </c>
-      <c r="AC8" s="2">
+      <c r="AC8" s="4">
         <v>25.5</v>
       </c>
-      <c r="AD8" s="2">
+      <c r="AD8" s="4">
         <v>0.215</v>
       </c>
-      <c r="AE8" s="2">
+      <c r="AE8" s="4">
         <v>106.6</v>
       </c>
+      <c r="AF8" s="1"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+    <row r="9" spans="1:32">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
         <v>26.7</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="4">
         <v>223</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="4">
         <v>1229</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="4">
         <v>40.1</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="4">
         <v>88.5</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="4">
         <v>7.7</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="4">
         <v>21.5</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="4">
         <v>18</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="4">
         <v>23.9</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="4">
         <v>12</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="4">
         <v>33.4</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="4">
         <v>45.4</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="Q9" s="4">
         <v>23.9</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R9" s="4">
         <v>8.4</v>
       </c>
-      <c r="S9" s="2">
+      <c r="S9" s="4">
         <v>5.5</v>
       </c>
-      <c r="T9" s="2">
+      <c r="T9" s="4">
         <v>15.7</v>
       </c>
-      <c r="U9" s="2">
+      <c r="U9" s="4">
         <v>21.4</v>
       </c>
-      <c r="V9" s="2">
+      <c r="V9" s="4">
         <v>105.8</v>
       </c>
-      <c r="W9" s="2">
+      <c r="W9" s="4">
         <v>0.45300000000000001</v>
       </c>
-      <c r="X9" s="2">
+      <c r="X9" s="4">
         <v>0.35899999999999999</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="Y9" s="4">
         <v>0.753</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="Z9" s="4">
         <v>92</v>
       </c>
-      <c r="AA9" s="2">
+      <c r="AA9" s="4">
         <v>0.496</v>
       </c>
-      <c r="AB9" s="2">
+      <c r="AB9" s="4">
         <v>13.7</v>
       </c>
-      <c r="AC9" s="2">
+      <c r="AC9" s="4">
         <v>26.5</v>
       </c>
-      <c r="AD9" s="2">
+      <c r="AD9" s="4">
         <v>0.20399999999999999</v>
       </c>
-      <c r="AE9" s="2">
+      <c r="AE9" s="4">
         <v>105.8</v>
       </c>
+      <c r="AF9" s="1"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+    <row r="10" spans="1:32">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="4">
         <v>26.6</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="4">
         <v>223</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="4">
         <v>990</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="4">
         <v>39.6</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="4">
         <v>88.5</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="4">
         <v>7</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="4">
         <v>20</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="4">
         <v>18.399999999999999</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10" s="4">
         <v>24.4</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10" s="4">
         <v>12.4</v>
       </c>
-      <c r="O10" s="2">
+      <c r="O10" s="4">
         <v>33.5</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10" s="4">
         <v>45.8</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="Q10" s="4">
         <v>22.8</v>
       </c>
-      <c r="R10" s="2">
+      <c r="R10" s="4">
         <v>8.3000000000000007</v>
       </c>
-      <c r="S10" s="2">
+      <c r="S10" s="4">
         <v>5.5</v>
       </c>
-      <c r="T10" s="2">
+      <c r="T10" s="4">
         <v>15.8</v>
       </c>
-      <c r="U10" s="2">
+      <c r="U10" s="4">
         <v>21.3</v>
       </c>
-      <c r="V10" s="2">
+      <c r="V10" s="4">
         <v>104.6</v>
       </c>
-      <c r="W10" s="2">
+      <c r="W10" s="4">
         <v>0.44800000000000001</v>
       </c>
-      <c r="X10" s="2">
+      <c r="X10" s="4">
         <v>0.34899999999999998</v>
       </c>
-      <c r="Y10" s="2">
+      <c r="Y10" s="4">
         <v>0.752</v>
       </c>
-      <c r="Z10" s="2">
+      <c r="Z10" s="4">
         <v>91.3</v>
       </c>
-      <c r="AA10" s="2">
+      <c r="AA10" s="4">
         <v>0.48699999999999999</v>
       </c>
-      <c r="AB10" s="2">
+      <c r="AB10" s="4">
         <v>13.8</v>
       </c>
-      <c r="AC10" s="2">
+      <c r="AC10" s="4">
         <v>27</v>
       </c>
-      <c r="AD10" s="2">
+      <c r="AD10" s="4">
         <v>0.20799999999999999</v>
       </c>
-      <c r="AE10" s="2">
+      <c r="AE10" s="4">
         <v>104.6</v>
       </c>
+      <c r="AF10" s="1"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+    <row r="11" spans="1:32">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="4">
         <v>26.6</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="4">
         <v>223</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="4">
         <v>1230</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="4">
         <v>40.1</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="4">
         <v>87.5</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="4">
         <v>7</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="4">
         <v>19.399999999999999</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="4">
         <v>20</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="4">
         <v>26.3</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="4">
         <v>11.8</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="4">
         <v>32.799999999999997</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11" s="4">
         <v>44.6</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="Q11" s="4">
         <v>23.2</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R11" s="4">
         <v>7.9</v>
       </c>
-      <c r="S11" s="2">
+      <c r="S11" s="4">
         <v>5.2</v>
       </c>
-      <c r="T11" s="2">
+      <c r="T11" s="4">
         <v>15.4</v>
       </c>
-      <c r="U11" s="2">
+      <c r="U11" s="4">
         <v>22.3</v>
       </c>
-      <c r="V11" s="2">
+      <c r="V11" s="4">
         <v>107.3</v>
       </c>
-      <c r="W11" s="2">
+      <c r="W11" s="4">
         <v>0.45900000000000002</v>
       </c>
-      <c r="X11" s="2">
+      <c r="X11" s="4">
         <v>0.35799999999999998</v>
       </c>
-      <c r="Y11" s="2">
+      <c r="Y11" s="4">
         <v>0.76300000000000001</v>
       </c>
-      <c r="Z11" s="2">
+      <c r="Z11" s="4">
         <v>92.1</v>
       </c>
-      <c r="AA11" s="2">
+      <c r="AA11" s="4">
         <v>0.498</v>
       </c>
-      <c r="AB11" s="2">
+      <c r="AB11" s="4">
         <v>13.4</v>
       </c>
-      <c r="AC11" s="2">
+      <c r="AC11" s="4">
         <v>26.4</v>
       </c>
-      <c r="AD11" s="2">
+      <c r="AD11" s="4">
         <v>0.22900000000000001</v>
       </c>
-      <c r="AE11" s="2">
+      <c r="AE11" s="4">
         <v>107.3</v>
       </c>
+      <c r="AF11" s="1"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+    <row r="12" spans="1:32">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="4">
         <v>26.6</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="4">
         <v>222</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="4">
         <v>1230</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="4">
         <v>40.4</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="4">
         <v>87.5</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="4">
         <v>6.9</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="4">
         <v>19.399999999999999</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="4">
         <v>19.899999999999999</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="4">
         <v>26.3</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="4">
         <v>11.7</v>
       </c>
-      <c r="O12" s="2">
+      <c r="O12" s="4">
         <v>32.9</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12" s="4">
         <v>44.7</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="Q12" s="4">
         <v>22.8</v>
       </c>
-      <c r="R12" s="2">
+      <c r="R12" s="4">
         <v>7.7</v>
       </c>
-      <c r="S12" s="2">
+      <c r="S12" s="4">
         <v>5.2</v>
       </c>
-      <c r="T12" s="2">
+      <c r="T12" s="4">
         <v>15.2</v>
       </c>
-      <c r="U12" s="2">
+      <c r="U12" s="4">
         <v>22.3</v>
       </c>
-      <c r="V12" s="2">
+      <c r="V12" s="4">
         <v>107.6</v>
       </c>
-      <c r="W12" s="2">
+      <c r="W12" s="4">
         <v>0.46100000000000002</v>
       </c>
-      <c r="X12" s="2">
+      <c r="X12" s="4">
         <v>0.35499999999999998</v>
       </c>
-      <c r="Y12" s="2">
+      <c r="Y12" s="4">
         <v>0.75900000000000001</v>
       </c>
-      <c r="Z12" s="2">
+      <c r="Z12" s="4">
         <v>92.7</v>
       </c>
-      <c r="AA12" s="2">
+      <c r="AA12" s="4">
         <v>0.501</v>
       </c>
-      <c r="AB12" s="2">
+      <c r="AB12" s="4">
         <v>13.3</v>
       </c>
-      <c r="AC12" s="2">
+      <c r="AC12" s="4">
         <v>26.3</v>
       </c>
-      <c r="AD12" s="2">
+      <c r="AD12" s="4">
         <v>0.22800000000000001</v>
       </c>
-      <c r="AE12" s="2">
+      <c r="AE12" s="4">
         <v>107.6</v>
       </c>
+      <c r="AF12" s="1"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+    <row r="13" spans="1:32">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="4">
         <v>26.6</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="4">
         <v>221</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="4">
         <v>1230</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="4">
         <v>40.200000000000003</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="4">
         <v>87.7</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="4">
         <v>7.2</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="4">
         <v>19.600000000000001</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="4">
         <v>20.7</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="4">
         <v>26.8</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="4">
         <v>12</v>
       </c>
-      <c r="O13" s="2">
+      <c r="O13" s="4">
         <v>32.799999999999997</v>
       </c>
-      <c r="P13" s="2">
+      <c r="P13" s="4">
         <v>44.7</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="Q13" s="4">
         <v>22.7</v>
       </c>
-      <c r="R13" s="2">
+      <c r="R13" s="4">
         <v>7.9</v>
       </c>
-      <c r="S13" s="2">
+      <c r="S13" s="4">
         <v>5.2</v>
       </c>
-      <c r="T13" s="2">
+      <c r="T13" s="4">
         <v>15.2</v>
       </c>
-      <c r="U13" s="2">
+      <c r="U13" s="4">
         <v>22.8</v>
       </c>
-      <c r="V13" s="2">
+      <c r="V13" s="4">
         <v>108.3</v>
       </c>
-      <c r="W13" s="2">
+      <c r="W13" s="4">
         <v>0.45900000000000002</v>
       </c>
-      <c r="X13" s="2">
+      <c r="X13" s="4">
         <v>0.36699999999999999</v>
       </c>
-      <c r="Y13" s="2">
+      <c r="Y13" s="4">
         <v>0.77100000000000002</v>
       </c>
-      <c r="Z13" s="2">
+      <c r="Z13" s="4">
         <v>91.7</v>
       </c>
-      <c r="AA13" s="2">
+      <c r="AA13" s="4">
         <v>0.5</v>
       </c>
-      <c r="AB13" s="2">
+      <c r="AB13" s="4">
         <v>13.3</v>
       </c>
-      <c r="AC13" s="2">
+      <c r="AC13" s="4">
         <v>26.7</v>
       </c>
-      <c r="AD13" s="2">
+      <c r="AD13" s="4">
         <v>0.23599999999999999</v>
       </c>
-      <c r="AE13" s="2">
+      <c r="AE13" s="4">
         <v>108.3</v>
       </c>
+      <c r="AF13" s="1"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+    <row r="14" spans="1:32">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="4">
         <v>26.8</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="4">
         <v>220</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="4">
         <v>1230</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="4">
         <v>40.1</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="4">
         <v>87.7</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="4">
         <v>7.1</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="4">
         <v>19.5</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="4">
         <v>20.3</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="4">
         <v>26.8</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="4">
         <v>12</v>
       </c>
-      <c r="O14" s="2">
+      <c r="O14" s="4">
         <v>33.1</v>
       </c>
-      <c r="P14" s="2">
+      <c r="P14" s="4">
         <v>45.2</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="Q14" s="4">
         <v>23.4</v>
       </c>
-      <c r="R14" s="2">
+      <c r="R14" s="4">
         <v>7.8</v>
       </c>
-      <c r="S14" s="2">
+      <c r="S14" s="4">
         <v>5.0999999999999996</v>
       </c>
-      <c r="T14" s="2">
+      <c r="T14" s="4">
         <v>15.2</v>
       </c>
-      <c r="U14" s="2">
+      <c r="U14" s="4">
         <v>22.6</v>
       </c>
-      <c r="V14" s="2">
+      <c r="V14" s="4">
         <v>107.5</v>
       </c>
-      <c r="W14" s="2">
+      <c r="W14" s="4">
         <v>0.45700000000000002</v>
       </c>
-      <c r="X14" s="2">
+      <c r="X14" s="4">
         <v>0.36199999999999999</v>
       </c>
-      <c r="Y14" s="2">
+      <c r="Y14" s="4">
         <v>0.755</v>
       </c>
-      <c r="Z14" s="2">
+      <c r="Z14" s="4">
         <v>92.4</v>
       </c>
-      <c r="AA14" s="2">
+      <c r="AA14" s="4">
         <v>0.497</v>
       </c>
-      <c r="AB14" s="2">
+      <c r="AB14" s="4">
         <v>13.2</v>
       </c>
-      <c r="AC14" s="2">
+      <c r="AC14" s="4">
         <v>26.7</v>
       </c>
-      <c r="AD14" s="2">
+      <c r="AD14" s="4">
         <v>0.23100000000000001</v>
       </c>
-      <c r="AE14" s="2">
+      <c r="AE14" s="4">
         <v>107.5</v>
       </c>
+      <c r="AF14" s="1"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+    <row r="15" spans="1:32">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="4">
         <v>26.6</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="4">
         <v>219</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="4">
         <v>1230</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="4">
         <v>39.4</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="4">
         <v>85.9</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="4">
         <v>6.5</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="4">
         <v>18.3</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="4">
         <v>21.1</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="4">
         <v>28.1</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="4">
         <v>12</v>
       </c>
-      <c r="O15" s="2">
+      <c r="O15" s="4">
         <v>32.299999999999997</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P15" s="4">
         <v>44.3</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="Q15" s="4">
         <v>22.9</v>
       </c>
-      <c r="R15" s="2">
+      <c r="R15" s="4">
         <v>7.8</v>
       </c>
-      <c r="S15" s="2">
+      <c r="S15" s="4">
         <v>5</v>
       </c>
-      <c r="T15" s="2">
+      <c r="T15" s="4">
         <v>16.3</v>
       </c>
-      <c r="U15" s="2">
+      <c r="U15" s="4">
         <v>24</v>
       </c>
-      <c r="V15" s="2">
+      <c r="V15" s="4">
         <v>106.5</v>
       </c>
-      <c r="W15" s="2">
+      <c r="W15" s="4">
         <v>0.45800000000000002</v>
       </c>
-      <c r="X15" s="2">
+      <c r="X15" s="4">
         <v>0.35799999999999998</v>
       </c>
-      <c r="Y15" s="2">
+      <c r="Y15" s="4">
         <v>0.752</v>
       </c>
-      <c r="Z15" s="2">
+      <c r="Z15" s="4">
         <v>91.9</v>
       </c>
-      <c r="AA15" s="2">
+      <c r="AA15" s="4">
         <v>0.496</v>
       </c>
-      <c r="AB15" s="2">
+      <c r="AB15" s="4">
         <v>14.2</v>
       </c>
-      <c r="AC15" s="2">
+      <c r="AC15" s="4">
         <v>27.1</v>
       </c>
-      <c r="AD15" s="2">
+      <c r="AD15" s="4">
         <v>0.246</v>
       </c>
-      <c r="AE15" s="2">
+      <c r="AE15" s="4">
         <v>106.5</v>
       </c>
+      <c r="AF15" s="1"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+    <row r="16" spans="1:32">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <v>26.5</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="4">
         <v>220</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="4">
         <v>1230</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="4">
         <v>39.200000000000003</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="4">
         <v>86.5</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="4">
         <v>6.3</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="4">
         <v>17.5</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="4">
         <v>21.5</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="4">
         <v>28.8</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16" s="4">
         <v>12.2</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O16" s="4">
         <v>32.6</v>
       </c>
-      <c r="P16" s="2">
+      <c r="P16" s="4">
         <v>44.8</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="Q16" s="4">
         <v>22.6</v>
       </c>
-      <c r="R16" s="2">
+      <c r="R16" s="4">
         <v>7.8</v>
       </c>
-      <c r="S16" s="2">
+      <c r="S16" s="4">
         <v>5.0999999999999996</v>
       </c>
-      <c r="T16" s="2">
+      <c r="T16" s="4">
         <v>15.8</v>
       </c>
-      <c r="U16" s="2">
+      <c r="U16" s="4">
         <v>24.9</v>
       </c>
-      <c r="V16" s="2">
+      <c r="V16" s="4">
         <v>106.2</v>
       </c>
-      <c r="W16" s="2">
+      <c r="W16" s="4">
         <v>0.45400000000000001</v>
       </c>
-      <c r="X16" s="2">
+      <c r="X16" s="4">
         <v>0.35799999999999998</v>
       </c>
-      <c r="Y16" s="2">
+      <c r="Y16" s="4">
         <v>0.745</v>
       </c>
-      <c r="Z16" s="2">
+      <c r="Z16" s="4">
         <v>90.5</v>
       </c>
-      <c r="AA16" s="2">
+      <c r="AA16" s="4">
         <v>0.49</v>
       </c>
-      <c r="AB16" s="2">
+      <c r="AB16" s="4">
         <v>13.7</v>
       </c>
-      <c r="AC16" s="2">
+      <c r="AC16" s="4">
         <v>27.3</v>
       </c>
-      <c r="AD16" s="2">
+      <c r="AD16" s="4">
         <v>0.248</v>
       </c>
-      <c r="AE16" s="2">
+      <c r="AE16" s="4">
         <v>106.2</v>
       </c>
+      <c r="AF16" s="1"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+    <row r="17" spans="1:32">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="4">
         <v>26.9</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="4">
         <v>220</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="4">
         <v>1230</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="4">
         <v>39.200000000000003</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="4">
         <v>87.7</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="4">
         <v>6.1</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="4">
         <v>17.2</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="4">
         <v>21.5</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M17" s="4">
         <v>28.4</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N17" s="4">
         <v>13.1</v>
       </c>
-      <c r="O17" s="2">
+      <c r="O17" s="4">
         <v>32.6</v>
       </c>
-      <c r="P17" s="2">
+      <c r="P17" s="4">
         <v>45.7</v>
       </c>
-      <c r="Q17" s="2">
+      <c r="Q17" s="4">
         <v>23.2</v>
       </c>
-      <c r="R17" s="2">
+      <c r="R17" s="4">
         <v>8.1999999999999993</v>
       </c>
-      <c r="S17" s="2">
+      <c r="S17" s="4">
         <v>5.3</v>
       </c>
-      <c r="T17" s="2">
+      <c r="T17" s="4">
         <v>15.8</v>
       </c>
-      <c r="U17" s="2">
+      <c r="U17" s="4">
         <v>24.7</v>
       </c>
-      <c r="V17" s="2">
+      <c r="V17" s="4">
         <v>106.1</v>
       </c>
-      <c r="W17" s="2">
+      <c r="W17" s="4">
         <v>0.44700000000000001</v>
       </c>
-      <c r="X17" s="2">
+      <c r="X17" s="4">
         <v>0.35599999999999998</v>
       </c>
-      <c r="Y17" s="2">
+      <c r="Y17" s="4">
         <v>0.75600000000000001</v>
       </c>
-      <c r="Z17" s="2">
+      <c r="Z17" s="4">
         <v>90.9</v>
       </c>
-      <c r="AA17" s="2">
+      <c r="AA17" s="4">
         <v>0.48199999999999998</v>
       </c>
-      <c r="AB17" s="2">
+      <c r="AB17" s="4">
         <v>13.6</v>
       </c>
-      <c r="AC17" s="2">
+      <c r="AC17" s="4">
         <v>28.7</v>
       </c>
-      <c r="AD17" s="2">
+      <c r="AD17" s="4">
         <v>0.245</v>
       </c>
-      <c r="AE17" s="2">
+      <c r="AE17" s="4">
         <v>106.1</v>
       </c>
+      <c r="AF17" s="1"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+    <row r="18" spans="1:32">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="4">
         <v>27</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="4">
         <v>219</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="4">
         <v>1189</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="4">
         <v>38.6</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="4">
         <v>88</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="4">
         <v>5.7</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="4">
         <v>16.399999999999999</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="4">
         <v>20.100000000000001</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M18" s="4">
         <v>26.7</v>
       </c>
-      <c r="N18" s="2">
+      <c r="N18" s="4">
         <v>13.3</v>
       </c>
-      <c r="O18" s="2">
+      <c r="O18" s="4">
         <v>33.200000000000003</v>
       </c>
-      <c r="P18" s="2">
+      <c r="P18" s="4">
         <v>46.5</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="Q18" s="4">
         <v>23.5</v>
       </c>
-      <c r="R18" s="2">
+      <c r="R18" s="4">
         <v>8.6999999999999993</v>
       </c>
-      <c r="S18" s="2">
+      <c r="S18" s="4">
         <v>5.6</v>
       </c>
-      <c r="T18" s="2">
+      <c r="T18" s="4">
         <v>16.5</v>
       </c>
-      <c r="U18" s="2">
+      <c r="U18" s="4">
         <v>23.6</v>
       </c>
-      <c r="V18" s="2">
+      <c r="V18" s="4">
         <v>102.9</v>
       </c>
-      <c r="W18" s="2">
+      <c r="W18" s="4">
         <v>0.439</v>
       </c>
-      <c r="X18" s="2">
+      <c r="X18" s="4">
         <v>0.34699999999999998</v>
       </c>
-      <c r="Y18" s="2">
+      <c r="Y18" s="4">
         <v>0.752</v>
       </c>
-      <c r="Z18" s="2">
+      <c r="Z18" s="4">
         <v>90.1</v>
       </c>
-      <c r="AA18" s="2">
+      <c r="AA18" s="4">
         <v>0.47099999999999997</v>
       </c>
-      <c r="AB18" s="2">
+      <c r="AB18" s="4">
         <v>14.2</v>
       </c>
-      <c r="AC18" s="2">
+      <c r="AC18" s="4">
         <v>28.6</v>
       </c>
-      <c r="AD18" s="2">
+      <c r="AD18" s="4">
         <v>0.22800000000000001</v>
       </c>
-      <c r="AE18" s="2">
+      <c r="AE18" s="4">
         <v>102.9</v>
       </c>
+      <c r="AF18" s="1"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+    <row r="19" spans="1:32">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="4">
         <v>27.2</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="4">
         <v>219</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="4">
         <v>1189</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="4">
         <v>38.9</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="4">
         <v>88.1</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="4">
         <v>5.6</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="4">
         <v>16</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L19" s="4">
         <v>20.2</v>
       </c>
-      <c r="M19" s="2">
+      <c r="M19" s="4">
         <v>26.6</v>
       </c>
-      <c r="N19" s="2">
+      <c r="N19" s="4">
         <v>13.1</v>
       </c>
-      <c r="O19" s="2">
+      <c r="O19" s="4">
         <v>33</v>
       </c>
-      <c r="P19" s="2">
+      <c r="P19" s="4">
         <v>46.1</v>
       </c>
-      <c r="Q19" s="2">
+      <c r="Q19" s="4">
         <v>23.4</v>
       </c>
-      <c r="R19" s="2">
+      <c r="R19" s="4">
         <v>8.6999999999999993</v>
       </c>
-      <c r="S19" s="2">
+      <c r="S19" s="4">
         <v>5.5</v>
       </c>
-      <c r="T19" s="2">
+      <c r="T19" s="4">
         <v>16.3</v>
       </c>
-      <c r="U19" s="2">
+      <c r="U19" s="4">
         <v>23.7</v>
       </c>
-      <c r="V19" s="2">
+      <c r="V19" s="4">
         <v>103.6</v>
       </c>
-      <c r="W19" s="2">
+      <c r="W19" s="4">
         <v>0.442</v>
       </c>
-      <c r="X19" s="2">
+      <c r="X19" s="4">
         <v>0.34899999999999998</v>
       </c>
-      <c r="Y19" s="2">
+      <c r="Y19" s="4">
         <v>0.75800000000000001</v>
       </c>
-      <c r="Z19" s="2">
+      <c r="Z19" s="4">
         <v>91</v>
       </c>
-      <c r="AA19" s="2">
+      <c r="AA19" s="4">
         <v>0.47399999999999998</v>
       </c>
-      <c r="AB19" s="2">
+      <c r="AB19" s="4">
         <v>14</v>
       </c>
-      <c r="AC19" s="2">
+      <c r="AC19" s="4">
         <v>28.5</v>
       </c>
-      <c r="AD19" s="2">
+      <c r="AD19" s="4">
         <v>0.22900000000000001</v>
       </c>
-      <c r="AE19" s="2">
+      <c r="AE19" s="4">
         <v>103.6</v>
       </c>
+      <c r="AF19" s="1"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+    <row r="20" spans="1:32">
+      <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="4">
         <v>27.4</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="4">
         <v>218</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="4">
         <v>1189</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="4">
         <v>39.6</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="4">
         <v>89</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="4">
         <v>5.7</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="4">
         <v>16.100000000000001</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L20" s="4">
         <v>19.600000000000001</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20" s="4">
         <v>26.1</v>
       </c>
-      <c r="N20" s="2">
+      <c r="N20" s="4">
         <v>13.4</v>
       </c>
-      <c r="O20" s="2">
+      <c r="O20" s="4">
         <v>33</v>
       </c>
-      <c r="P20" s="2">
+      <c r="P20" s="4">
         <v>46.4</v>
       </c>
-      <c r="Q20" s="2">
+      <c r="Q20" s="4">
         <v>24</v>
       </c>
-      <c r="R20" s="2">
+      <c r="R20" s="4">
         <v>8.5</v>
       </c>
-      <c r="S20" s="2">
+      <c r="S20" s="4">
         <v>5.7</v>
       </c>
-      <c r="T20" s="2">
+      <c r="T20" s="4">
         <v>15.8</v>
       </c>
-      <c r="U20" s="2">
+      <c r="U20" s="4">
         <v>23.2</v>
       </c>
-      <c r="V20" s="2">
+      <c r="V20" s="4">
         <v>104.5</v>
       </c>
-      <c r="W20" s="2">
+      <c r="W20" s="4">
         <v>0.44500000000000001</v>
       </c>
-      <c r="X20" s="2">
+      <c r="X20" s="4">
         <v>0.35399999999999998</v>
       </c>
-      <c r="Y20" s="2">
+      <c r="Y20" s="4">
         <v>0.752</v>
       </c>
-      <c r="Z20" s="2">
+      <c r="Z20" s="4">
         <v>90.7</v>
       </c>
-      <c r="AA20" s="2">
+      <c r="AA20" s="4">
         <v>0.47699999999999998</v>
       </c>
-      <c r="AB20" s="2">
+      <c r="AB20" s="4">
         <v>13.6</v>
       </c>
-      <c r="AC20" s="2">
+      <c r="AC20" s="4">
         <v>28.9</v>
       </c>
-      <c r="AD20" s="2">
+      <c r="AD20" s="4">
         <v>0.221</v>
       </c>
-      <c r="AE20" s="2">
+      <c r="AE20" s="4">
         <v>104.5</v>
       </c>
+      <c r="AF20" s="1"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+    <row r="21" spans="1:32">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="4">
         <v>27.7</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="4">
         <v>216</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="4">
         <v>1189</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="4">
         <v>38.799999999999997</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="4">
         <v>87.6</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" s="4">
         <v>5.3</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="4">
         <v>14.9</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L21" s="4">
         <v>20.2</v>
       </c>
-      <c r="M21" s="2">
+      <c r="M21" s="4">
         <v>27</v>
       </c>
-      <c r="N21" s="2">
+      <c r="N21" s="4">
         <v>13</v>
       </c>
-      <c r="O21" s="2">
+      <c r="O21" s="4">
         <v>33.1</v>
       </c>
-      <c r="P21" s="2">
+      <c r="P21" s="4">
         <v>46.1</v>
       </c>
-      <c r="Q21" s="2">
+      <c r="Q21" s="4">
         <v>23.7</v>
       </c>
-      <c r="R21" s="2">
+      <c r="R21" s="4">
         <v>8.5</v>
       </c>
-      <c r="S21" s="2">
+      <c r="S21" s="4">
         <v>5.7</v>
       </c>
-      <c r="T21" s="2">
+      <c r="T21" s="4">
         <v>16.399999999999999</v>
       </c>
-      <c r="U21" s="2">
+      <c r="U21" s="4">
         <v>24.3</v>
       </c>
-      <c r="V21" s="2">
+      <c r="V21" s="4">
         <v>103</v>
       </c>
-      <c r="W21" s="2">
+      <c r="W21" s="4">
         <v>0.443</v>
       </c>
-      <c r="X21" s="2">
+      <c r="X21" s="4">
         <v>0.35399999999999998</v>
       </c>
-      <c r="Y21" s="2">
+      <c r="Y21" s="4">
         <v>0.748</v>
       </c>
-      <c r="Z21" s="2">
+      <c r="Z21" s="4">
         <v>91.3</v>
       </c>
-      <c r="AA21" s="2">
+      <c r="AA21" s="4">
         <v>0.47299999999999998</v>
       </c>
-      <c r="AB21" s="2">
+      <c r="AB21" s="4">
         <v>14.1</v>
       </c>
-      <c r="AC21" s="2">
+      <c r="AC21" s="4">
         <v>28.2</v>
       </c>
-      <c r="AD21" s="2">
+      <c r="AD21" s="4">
         <v>0.23100000000000001</v>
       </c>
-      <c r="AE21" s="2">
+      <c r="AE21" s="4">
         <v>10</v>
       </c>
+      <c r="AF21" s="1"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="E23" s="5"/>
+    <row r="22" spans="1:32">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="E24" s="5"/>
+    <row r="23" spans="1:32">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+      <c r="AF23" s="1"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="E25" s="5"/>
+    <row r="24" spans="1:32">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="1"/>
+      <c r="AF24" s="1"/>
+    </row>
+    <row r="25" spans="1:32">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+      <c r="AF25" s="1"/>
+    </row>
+    <row r="26" spans="1:32">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="1"/>
+      <c r="AF26" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>